<commit_message>
Phase 2 Constellation Launches
Updated scenarios.csv, scenarios_percs.xlsx, and inputs.py to increase the number of satellites by an order of magnitude. Reran the other scripts to adjust processed data & results files accordingly. Updated the R files to adjust for the change in scale of the data where necessary. Reran all R files to generate updated figures.
</commit_message>
<xml_diff>
--- a/data/raw/scenarios_percs.xlsx
+++ b/data/raw/scenarios_percs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoughton\Desktop\Github\saleos\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rushi\saleos\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CB9D32-08D3-416B-9418-D0F589890798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7206BE4-012F-4F98-B594-C3A8CF301042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios copy" sheetId="1" r:id="rId1"/>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H2:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,8 +1068,8 @@
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="H2">
-        <v>4425</v>
+      <c r="H2" s="1">
+        <v>44250</v>
       </c>
       <c r="I2">
         <v>127</v>
@@ -1119,8 +1119,8 @@
       <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3">
-        <v>394</v>
+      <c r="H3" s="1">
+        <v>3940</v>
       </c>
       <c r="I3">
         <v>14</v>
@@ -1168,8 +1168,8 @@
       <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="H4">
-        <v>180</v>
+      <c r="H4" s="1">
+        <v>1800</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -1205,8 +1205,8 @@
       <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="H5">
-        <v>72</v>
+      <c r="H5" s="1">
+        <v>720</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -1250,8 +1250,8 @@
       <c r="G6" t="s">
         <v>27</v>
       </c>
-      <c r="H6">
-        <v>648</v>
+      <c r="H6" s="1">
+        <v>6480</v>
       </c>
       <c r="I6">
         <v>18</v>
@@ -1301,8 +1301,8 @@
       <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
-        <v>972</v>
+      <c r="H7" s="1">
+        <v>9720</v>
       </c>
       <c r="I7">
         <v>27</v>
@@ -1350,8 +1350,8 @@
       <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="H8">
-        <v>1368</v>
+      <c r="H8" s="1">
+        <v>13680</v>
       </c>
       <c r="I8">
         <v>38</v>
@@ -1382,8 +1382,8 @@
       <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="H9">
-        <v>108</v>
+      <c r="H9" s="1">
+        <v>1080</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -1414,8 +1414,8 @@
       <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="H10">
-        <v>72</v>
+      <c r="H10" s="1">
+        <v>720</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -1446,8 +1446,8 @@
       <c r="G11" t="s">
         <v>27</v>
       </c>
-      <c r="H11">
-        <v>72</v>
+      <c r="H11" s="1">
+        <v>720</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -1478,8 +1478,8 @@
       <c r="G12" t="s">
         <v>18</v>
       </c>
-      <c r="H12">
-        <v>10</v>
+      <c r="H12" s="1">
+        <v>100</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -1510,7 +1510,7 @@
       <c r="G13" t="s">
         <v>27</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>9</v>
       </c>
       <c r="I13">
@@ -1542,8 +1542,8 @@
       <c r="G14" t="s">
         <v>27</v>
       </c>
-      <c r="H14">
-        <v>4425</v>
+      <c r="H14" s="1">
+        <v>44250</v>
       </c>
       <c r="I14">
         <v>192</v>
@@ -1574,8 +1574,8 @@
       <c r="G15" t="s">
         <v>27</v>
       </c>
-      <c r="H15">
-        <v>648</v>
+      <c r="H15" s="1">
+        <v>6480</v>
       </c>
       <c r="I15">
         <v>18</v>
@@ -1606,8 +1606,8 @@
       <c r="G16" t="s">
         <v>27</v>
       </c>
-      <c r="H16">
-        <v>3236</v>
+      <c r="H16" s="1">
+        <v>32360</v>
       </c>
       <c r="I16">
         <v>90</v>
@@ -1638,8 +1638,8 @@
       <c r="G17" t="s">
         <v>27</v>
       </c>
-      <c r="H17">
-        <v>19</v>
+      <c r="H17" s="1">
+        <v>190</v>
       </c>
       <c r="I17">
         <v>19</v>
@@ -1670,8 +1670,8 @@
       <c r="G18" t="s">
         <v>18</v>
       </c>
-      <c r="H18">
-        <v>4425</v>
+      <c r="H18" s="1">
+        <v>44250</v>
       </c>
       <c r="I18">
         <v>192</v>
@@ -1702,8 +1702,8 @@
       <c r="G19" t="s">
         <v>18</v>
       </c>
-      <c r="H19">
-        <v>648</v>
+      <c r="H19" s="1">
+        <v>6480</v>
       </c>
       <c r="I19">
         <v>18</v>
@@ -1734,8 +1734,8 @@
       <c r="G20" t="s">
         <v>18</v>
       </c>
-      <c r="H20">
-        <v>3236</v>
+      <c r="H20" s="1">
+        <v>32360</v>
       </c>
       <c r="I20">
         <v>90</v>
@@ -1766,8 +1766,8 @@
       <c r="G21" t="s">
         <v>18</v>
       </c>
-      <c r="H21">
-        <v>19</v>
+      <c r="H21" s="1">
+        <v>190</v>
       </c>
       <c r="I21">
         <v>19</v>

</xml_diff>

<commit_message>
Minor formatting changes to code, vis scripts and figures file.
</commit_message>
<xml_diff>
--- a/data/raw/scenarios_percs.xlsx
+++ b/data/raw/scenarios_percs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoughton\Desktop\Github\saleos\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CB9D32-08D3-416B-9418-D0F589890798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235361B5-9460-441A-B801-D2989321CB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios copy" sheetId="1" r:id="rId1"/>
@@ -151,6 +151,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,10 +631,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -990,7 +994,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,15 +1266,15 @@
       <c r="L6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="3">
         <f>M2/$P$2</f>
         <v>0.62605042016806722</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="3">
         <f t="shared" ref="N6:O6" si="0">N2/$P$2</f>
         <v>0.35714285714285715</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="3">
         <f t="shared" si="0"/>
         <v>1.680672268907563E-2</v>
       </c>
@@ -1313,13 +1317,13 @@
       <c r="L7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="3">
         <f>O3/$P$3</f>
         <v>1</v>
       </c>

</xml_diff>